<commit_message>
set up order service
</commit_message>
<xml_diff>
--- a/task/task.xlsx
+++ b/task/task.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="OrderService" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="79">
   <si>
     <t>Task</t>
   </si>
@@ -207,12 +207,6 @@
     <t>should_return_201_when_post_comfirmation_success</t>
   </si>
   <si>
-    <t>should_return_201_when_patch_product_success</t>
-  </si>
-  <si>
-    <t>should_return_400_when_patch_product_fail</t>
-  </si>
-  <si>
     <t>should_return_201_when_patch_store_success</t>
   </si>
   <si>
@@ -240,12 +234,6 @@
     <t>should_return_400_when_post_user_fail</t>
   </si>
   <si>
-    <t>should_return_201_when_patch_user_success</t>
-  </si>
-  <si>
-    <t>should_return_400_when_patch_user_fail</t>
-  </si>
-  <si>
     <t>should_return_200_when_get_user_success</t>
   </si>
   <si>
@@ -271,6 +259,24 @@
   </si>
   <si>
     <t>launch docker and build images</t>
+  </si>
+  <si>
+    <t>should_return_201_when_put_product_success</t>
+  </si>
+  <si>
+    <t>should_return_400_when_put_product_fail</t>
+  </si>
+  <si>
+    <t>should_return_201_when_put_user_success</t>
+  </si>
+  <si>
+    <t>should_return_400_when_put_user_fail</t>
+  </si>
+  <si>
+    <t>should_return_201_when_put_cart_success</t>
+  </si>
+  <si>
+    <t>should_return_400_when_put_cart_fail</t>
   </si>
 </sst>
 </file>
@@ -345,12 +351,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -654,8 +663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -682,8 +691,8 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>70</v>
+      <c r="A2" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>16</v>
@@ -691,9 +700,12 @@
       <c r="C2" s="1">
         <v>5</v>
       </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
+      <c r="A3" s="4"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -702,7 +714,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
+      <c r="A4" s="4"/>
       <c r="B4" s="1" t="s">
         <v>18</v>
       </c>
@@ -711,7 +723,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
+      <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
         <v>20</v>
       </c>
@@ -720,7 +732,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
+      <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
@@ -729,7 +741,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
+      <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
@@ -738,7 +750,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
+      <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
@@ -747,7 +759,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
+      <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -756,7 +768,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
+      <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
@@ -765,7 +777,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
+      <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
@@ -774,7 +786,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
+      <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
         <v>21</v>
       </c>
@@ -783,7 +795,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
+      <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
@@ -792,7 +804,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="3"/>
+      <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
@@ -801,7 +813,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
+      <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
@@ -810,7 +822,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
+      <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
@@ -819,7 +831,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
+      <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
@@ -828,7 +840,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
+      <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
@@ -1010,8 +1022,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>70</v>
+      <c r="A9" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>31</v>
@@ -1021,7 +1033,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
+      <c r="A10" s="5"/>
       <c r="B10" s="1" t="s">
         <v>27</v>
       </c>
@@ -1030,7 +1042,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
+      <c r="A11" s="5"/>
       <c r="B11" s="1" t="s">
         <v>28</v>
       </c>
@@ -1039,7 +1051,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
+      <c r="A12" s="5"/>
       <c r="B12" s="1" t="s">
         <v>29</v>
       </c>
@@ -1048,7 +1060,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
+      <c r="A13" s="5"/>
       <c r="B13" s="1" t="s">
         <v>32</v>
       </c>
@@ -1057,7 +1069,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
+      <c r="A14" s="5"/>
       <c r="B14" s="1" t="s">
         <v>33</v>
       </c>
@@ -1066,7 +1078,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
+      <c r="A15" s="5"/>
       <c r="B15" s="1" t="s">
         <v>34</v>
       </c>
@@ -1075,7 +1087,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
+      <c r="A16" s="5"/>
       <c r="B16" s="1" t="s">
         <v>35</v>
       </c>
@@ -1084,18 +1096,18 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
+      <c r="A17" s="5"/>
       <c r="B17" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C17" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
+      <c r="A18" s="5"/>
       <c r="B18" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C18" s="1">
         <v>3</v>
@@ -1123,7 +1135,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="60" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1150,8 +1162,8 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>70</v>
+      <c r="A2" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>16</v>
@@ -1163,7 +1175,7 @@
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
+      <c r="A3" s="5"/>
       <c r="B3" s="1" t="s">
         <v>36</v>
       </c>
@@ -1172,7 +1184,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
+      <c r="A4" s="5"/>
       <c r="B4" s="1" t="s">
         <v>37</v>
       </c>
@@ -1181,7 +1193,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
+      <c r="A5" s="5"/>
       <c r="B5" s="1" t="s">
         <v>38</v>
       </c>
@@ -1190,7 +1202,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
+      <c r="A6" s="5"/>
       <c r="B6" s="1" t="s">
         <v>39</v>
       </c>
@@ -1199,7 +1211,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
+      <c r="A7" s="5"/>
       <c r="B7" s="1" t="s">
         <v>40</v>
       </c>
@@ -1208,18 +1220,18 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
+      <c r="A8" s="5"/>
       <c r="B8" s="1" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="C8" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
+      <c r="A9" s="5"/>
       <c r="B9" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="C9" s="1">
         <v>3</v>
@@ -1246,7 +1258,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -1274,8 +1286,8 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>70</v>
+      <c r="A2" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>16</v>
@@ -1285,7 +1297,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
+      <c r="A3" s="5"/>
       <c r="B3" s="1" t="s">
         <v>41</v>
       </c>
@@ -1294,7 +1306,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
+      <c r="A4" s="5"/>
       <c r="B4" s="1" t="s">
         <v>43</v>
       </c>
@@ -1303,7 +1315,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
+      <c r="A5" s="5"/>
       <c r="B5" s="1" t="s">
         <v>42</v>
       </c>
@@ -1312,7 +1324,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
+      <c r="A6" s="5"/>
       <c r="B6" s="1" t="s">
         <v>44</v>
       </c>
@@ -1377,8 +1389,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>70</v>
+      <c r="A3" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>45</v>
@@ -1388,7 +1400,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
+      <c r="A4" s="5"/>
       <c r="B4" s="1" t="s">
         <v>50</v>
       </c>
@@ -1397,7 +1409,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
+      <c r="A5" s="5"/>
       <c r="B5" s="1" t="s">
         <v>46</v>
       </c>
@@ -1406,7 +1418,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
+      <c r="A6" s="5"/>
       <c r="B6" s="1" t="s">
         <v>47</v>
       </c>
@@ -1415,7 +1427,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
+      <c r="A7" s="5"/>
       <c r="B7" s="1" t="s">
         <v>48</v>
       </c>
@@ -1424,7 +1436,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
+      <c r="A8" s="5"/>
       <c r="B8" s="1" t="s">
         <v>49</v>
       </c>
@@ -1433,7 +1445,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
+      <c r="A9" s="5"/>
       <c r="B9" s="1" t="s">
         <v>51</v>
       </c>
@@ -1442,7 +1454,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
+      <c r="A10" s="5"/>
       <c r="B10" s="1" t="s">
         <v>52</v>
       </c>
@@ -1451,7 +1463,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
+      <c r="A11" s="5"/>
       <c r="B11" s="1" t="s">
         <v>53</v>
       </c>
@@ -1460,7 +1472,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
+      <c r="A12" s="5"/>
       <c r="B12" s="1" t="s">
         <v>54</v>
       </c>
@@ -1469,7 +1481,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
+      <c r="A13" s="5"/>
       <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
@@ -1478,7 +1490,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
+      <c r="A14" s="5"/>
       <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
@@ -1505,10 +1517,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1535,8 +1547,8 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>70</v>
+      <c r="A2" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>16</v>
@@ -1546,62 +1558,80 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
+      <c r="A3" s="5"/>
       <c r="B3" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C3" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
+      <c r="A4" s="5"/>
       <c r="B4" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C4" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
+      <c r="A5" s="5"/>
       <c r="B5" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C5" s="1">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
+      <c r="A6" s="5"/>
       <c r="B6" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C6" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="1" t="s">
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="3" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="1">
-        <f>SUM(C2:C7)</f>
-        <v>39</v>
+      <c r="C10" s="1">
+        <f>SUM(C2:C9)</f>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A2:A9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1612,7 +1642,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1639,8 +1669,8 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>70</v>
+      <c r="A2" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>16</v>
@@ -1650,54 +1680,54 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
+      <c r="A3" s="5"/>
       <c r="B3" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C3" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
+      <c r="A4" s="5"/>
       <c r="B4" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C4" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
+      <c r="A5" s="5"/>
       <c r="B5" s="1" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="C5" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
+      <c r="A6" s="5"/>
       <c r="B6" s="1" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="C6" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
+      <c r="A7" s="5"/>
       <c r="B7" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C7" s="1">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
+      <c r="A8" s="5"/>
       <c r="B8" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C8" s="1">
         <v>3</v>
@@ -1752,7 +1782,7 @@
     </row>
     <row r="2" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B2" s="1">
         <v>10</v>
@@ -1760,7 +1790,7 @@
     </row>
     <row r="3" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B3" s="1">
         <v>15</v>
@@ -1768,7 +1798,7 @@
     </row>
     <row r="4" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B4" s="1">
         <v>15</v>
@@ -1776,7 +1806,7 @@
     </row>
     <row r="5" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B5" s="1">
         <v>10</v>
@@ -1784,7 +1814,7 @@
     </row>
     <row r="6" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B6" s="1">
         <v>30</v>
@@ -1792,7 +1822,7 @@
     </row>
     <row r="7" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B7" s="1">
         <v>40</v>

</xml_diff>

<commit_message>
add postOrderApi to order service
</commit_message>
<xml_diff>
--- a/task/task.xlsx
+++ b/task/task.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="80">
   <si>
     <t>Task</t>
   </si>
@@ -277,6 +277,9 @@
   </si>
   <si>
     <t>should_return_400_when_put_cart_fail</t>
+  </si>
+  <si>
+    <t>解决准备好模版中的bug</t>
   </si>
 </sst>
 </file>
@@ -332,8 +335,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -369,7 +374,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -378,6 +383,7 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -386,6 +392,7 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -664,7 +671,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -712,6 +719,12 @@
       <c r="C3" s="1">
         <v>10</v>
       </c>
+      <c r="D3" s="1">
+        <v>29</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
@@ -862,6 +875,7 @@
     <mergeCell ref="A2:A18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
set up price service
</commit_message>
<xml_diff>
--- a/task/task.xlsx
+++ b/task/task.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="OrderService" sheetId="1" r:id="rId1"/>
@@ -1313,7 +1313,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -1548,8 +1548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="60" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1582,6 +1582,9 @@
       <c r="C2" s="1">
         <v>5</v>
       </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -1700,6 +1703,10 @@
       <c r="C15" s="1">
         <f>SUM(C2:C14)</f>
         <v>89</v>
+      </c>
+      <c r="D15" s="1">
+        <f>SUM(D2:D14)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
set up cart service
</commit_message>
<xml_diff>
--- a/task/task.xlsx
+++ b/task/task.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="OrderService" sheetId="1" r:id="rId1"/>
@@ -1469,8 +1469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="60" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1748,8 +1748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1784,6 +1784,9 @@
       </c>
       <c r="C2" s="1">
         <v>5</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
set up inverntory service
</commit_message>
<xml_diff>
--- a/task/task.xlsx
+++ b/task/task.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" tabRatio="500" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="OrderService" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="96">
   <si>
     <t>Task</t>
   </si>
@@ -329,9 +329,6 @@
   </si>
   <si>
     <t>Service</t>
-  </si>
-  <si>
-    <t>第一个服务生疏</t>
   </si>
 </sst>
 </file>
@@ -1187,8 +1184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1225,9 +1222,6 @@
         <f>OrderService!D19</f>
         <v>190</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>96</v>
-      </c>
     </row>
     <row r="3" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="str">
@@ -1240,7 +1234,7 @@
       </c>
       <c r="C3" s="4">
         <f>InventoryService!D19</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1337,7 +1331,7 @@
       </c>
       <c r="C10" s="4">
         <f>SUM(C2:C9)</f>
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>
@@ -1349,8 +1343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1389,13 +1383,15 @@
       <c r="C2" s="2">
         <v>5</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1">
         <v>10</v>
@@ -1404,7 +1400,7 @@
     <row r="4" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C4" s="1">
         <v>3</v>
@@ -1413,7 +1409,7 @@
     <row r="5" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="1" t="s">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="C5" s="1">
         <v>8</v>
@@ -1422,7 +1418,7 @@
     <row r="6" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="1" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="C6" s="1">
         <v>8</v>
@@ -1431,7 +1427,7 @@
     <row r="7" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="1" t="s">
-        <v>77</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1">
         <v>3</v>
@@ -1440,7 +1436,7 @@
     <row r="8" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="C8" s="1">
         <v>10</v>
@@ -1449,7 +1445,7 @@
     <row r="9" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
       <c r="B9" s="1" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="C9" s="1">
         <v>3</v>
@@ -1458,61 +1454,61 @@
     <row r="10" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C10" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>75</v>
       </c>
       <c r="C12" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
       <c r="B13" s="1" t="s">
-        <v>27</v>
+        <v>76</v>
       </c>
       <c r="C13" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
       <c r="B14" s="1" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="C14" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
       <c r="B15" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C15" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="B16" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C16" s="1">
         <v>3</v>
@@ -1521,19 +1517,19 @@
     <row r="17" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
       <c r="B17" s="1" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="C17" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
       <c r="B18" s="1" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="C18" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1546,7 +1542,7 @@
       </c>
       <c r="D19" s="1">
         <f>SUM(D2:D18)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add post store api in inventoryService
</commit_message>
<xml_diff>
--- a/task/task.xlsx
+++ b/task/task.xlsx
@@ -384,8 +384,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="75">
+  <cellStyleXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -485,7 +489,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="75">
+  <cellStyles count="79">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -523,6 +527,8 @@
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -560,6 +566,8 @@
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1234,7 +1242,7 @@
       </c>
       <c r="C3" s="4">
         <f>InventoryService!D19</f>
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1331,7 +1339,7 @@
       </c>
       <c r="C10" s="4">
         <f>SUM(C2:C9)</f>
-        <v>309</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -1344,7 +1352,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1396,6 +1404,9 @@
       <c r="C3" s="1">
         <v>10</v>
       </c>
+      <c r="D3" s="1">
+        <v>13</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
@@ -1405,6 +1416,9 @@
       <c r="C4" s="1">
         <v>3</v>
       </c>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
@@ -1542,7 +1556,7 @@
       </c>
       <c r="D19" s="1">
         <f>SUM(D2:D18)</f>
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1550,6 +1564,7 @@
     <mergeCell ref="A2:A18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
set up refund service
</commit_message>
<xml_diff>
--- a/task/task.xlsx
+++ b/task/task.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="OrderService" sheetId="1" r:id="rId1"/>
@@ -1245,7 +1245,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1336,7 +1336,7 @@
       </c>
       <c r="C6" s="4">
         <f>RefundService!D15</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1391,7 +1391,7 @@
       </c>
       <c r="C10" s="4">
         <f>SUM(C2:C9)</f>
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
   </sheetData>
@@ -1403,7 +1403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -1909,7 +1909,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1950,7 +1950,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -2071,7 +2071,7 @@
       </c>
       <c r="D15" s="1">
         <f>SUM(D2:D14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
set up user service
</commit_message>
<xml_diff>
--- a/task/task.xlsx
+++ b/task/task.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" tabRatio="500" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="OrderService" sheetId="1" r:id="rId1"/>
@@ -1308,7 +1308,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -1434,7 +1434,7 @@
       </c>
       <c r="C8" s="4">
         <f>UserService!D9</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1461,7 +1461,7 @@
       </c>
       <c r="C10" s="4">
         <f>SUM(C2:C9)</f>
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
   </sheetData>
@@ -1980,7 +1980,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="60" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2368,7 +2368,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -2408,6 +2408,9 @@
       <c r="C2" s="1">
         <v>5</v>
       </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
@@ -2473,7 +2476,7 @@
       </c>
       <c r="D9" s="1">
         <f>SUM(D2:D8)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add service docker in docker-compose.yml
</commit_message>
<xml_diff>
--- a/task/task.xlsx
+++ b/task/task.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="99">
   <si>
     <t>Task</t>
   </si>
@@ -336,6 +336,9 @@
   </si>
   <si>
     <t>launch docker and debugging</t>
+  </si>
+  <si>
+    <t>拉docker时间未记入</t>
   </si>
 </sst>
 </file>
@@ -1469,7 +1472,7 @@
       </c>
       <c r="C9" s="4">
         <f>Docker!D6</f>
-        <v>28</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1482,7 +1485,7 @@
       </c>
       <c r="C10" s="4">
         <f>SUM(C2:C9)</f>
-        <v>555</v>
+        <v>571</v>
       </c>
     </row>
   </sheetData>
@@ -2532,7 +2535,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2584,6 +2587,12 @@
       <c r="C3" s="1">
         <v>15</v>
       </c>
+      <c r="D3" s="1">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6"/>
@@ -2593,6 +2602,9 @@
       <c r="C4" s="1">
         <v>10</v>
       </c>
+      <c r="E4" s="4" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
@@ -2613,7 +2625,7 @@
       </c>
       <c r="D6" s="1">
         <f>SUM(D2:D5)</f>
-        <v>28</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
launch docker and debugging
</commit_message>
<xml_diff>
--- a/task/task.xlsx
+++ b/task/task.xlsx
@@ -1472,7 +1472,7 @@
       </c>
       <c r="C9" s="4">
         <f>Docker!D6</f>
-        <v>44</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -1485,7 +1485,7 @@
       </c>
       <c r="C10" s="4">
         <f>SUM(C2:C9)</f>
-        <v>571</v>
+        <v>635</v>
       </c>
     </row>
   </sheetData>
@@ -2535,7 +2535,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2602,6 +2602,9 @@
       <c r="C4" s="1">
         <v>10</v>
       </c>
+      <c r="D4" s="1">
+        <v>6</v>
+      </c>
       <c r="E4" s="4" t="s">
         <v>98</v>
       </c>
@@ -2614,6 +2617,9 @@
       <c r="C5" s="1">
         <v>60</v>
       </c>
+      <c r="D5" s="1">
+        <v>58</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
@@ -2625,7 +2631,7 @@
       </c>
       <c r="D6" s="1">
         <f>SUM(D2:D5)</f>
-        <v>44</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish backend and docker
</commit_message>
<xml_diff>
--- a/task/task.xlsx
+++ b/task/task.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" tabRatio="500" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" tabRatio="500" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="OrderService" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="103">
   <si>
     <t>Task</t>
   </si>
@@ -342,6 +342,15 @@
   </si>
   <si>
     <t>add nginx</t>
+  </si>
+  <si>
+    <t>写shell脚本解决docker启动顺序问题</t>
+  </si>
+  <si>
+    <t>Extra</t>
+  </si>
+  <si>
+    <t>mysql docker数量由七个合为一个，使用不同数据库</t>
   </si>
 </sst>
 </file>
@@ -536,7 +545,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -551,6 +560,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -974,7 +986,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A27" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -1005,7 +1017,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>53</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1019,7 +1031,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
+      <c r="A3" s="7"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1034,7 +1046,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
@@ -1049,7 +1061,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
@@ -1064,7 +1076,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
@@ -1079,7 +1091,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
+      <c r="A7" s="7"/>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1094,7 +1106,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
+      <c r="A8" s="7"/>
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1106,7 +1118,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
+      <c r="A9" s="7"/>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1118,7 +1130,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
+      <c r="A10" s="7"/>
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1130,7 +1142,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
+      <c r="A11" s="7"/>
       <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1145,7 +1157,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6"/>
+      <c r="A12" s="7"/>
       <c r="B12" s="1" t="s">
         <v>17</v>
       </c>
@@ -1157,7 +1169,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
+      <c r="A13" s="7"/>
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
@@ -1169,7 +1181,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
+      <c r="A14" s="7"/>
       <c r="B14" s="1" t="s">
         <v>69</v>
       </c>
@@ -1181,7 +1193,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="6"/>
+      <c r="A15" s="7"/>
       <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
@@ -1193,7 +1205,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
+      <c r="A16" s="7"/>
       <c r="B16" s="1" t="s">
         <v>71</v>
       </c>
@@ -1205,7 +1217,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="6"/>
+      <c r="A17" s="7"/>
       <c r="B17" s="1" t="s">
         <v>72</v>
       </c>
@@ -1217,7 +1229,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="6"/>
+      <c r="A18" s="7"/>
       <c r="B18" s="1" t="s">
         <v>73</v>
       </c>
@@ -1254,7 +1266,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -1288,7 +1300,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1319,24 +1331,83 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T30" sqref="T30"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="36" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12" style="4" customWidth="1"/>
+    <col min="2" max="2" width="60" style="4" customWidth="1"/>
+    <col min="3" max="4" width="12" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="36" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="4">
+        <v>120</v>
+      </c>
+      <c r="D2" s="4">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="6">
+        <v>120</v>
+      </c>
+      <c r="D3" s="6">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4">
+        <f>SUM(C2:C3)</f>
+        <v>240</v>
+      </c>
+      <c r="D4" s="4">
+        <f>SUM(D2:D3)</f>
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1479,14 +1550,28 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="4" t="str">
+        <f>Extra!A1</f>
+        <v>Extra</v>
+      </c>
+      <c r="B10" s="4">
+        <f>Extra!C4</f>
+        <v>240</v>
+      </c>
+      <c r="C10" s="4">
+        <f>Extra!D4</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B11" s="4">
         <f>SUM(B2:B9)</f>
         <v>584</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C11" s="4">
         <f>SUM(C2:C9)</f>
         <v>649</v>
       </c>
@@ -1500,7 +1585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -1531,7 +1616,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>53</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1546,7 +1631,7 @@
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7"/>
+      <c r="A3" s="8"/>
       <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
@@ -1558,7 +1643,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="1" t="s">
         <v>24</v>
       </c>
@@ -1570,7 +1655,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="1" t="s">
         <v>25</v>
       </c>
@@ -1582,7 +1667,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="1" t="s">
         <v>26</v>
       </c>
@@ -1594,7 +1679,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
+      <c r="A7" s="8"/>
       <c r="B7" s="1" t="s">
         <v>27</v>
       </c>
@@ -1606,7 +1691,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="1" t="s">
         <v>86</v>
       </c>
@@ -1618,7 +1703,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="1" t="s">
         <v>87</v>
       </c>
@@ -1630,7 +1715,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
+      <c r="A10" s="8"/>
       <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
@@ -1642,7 +1727,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="7"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="1" t="s">
         <v>22</v>
       </c>
@@ -1654,7 +1739,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="7"/>
+      <c r="A12" s="8"/>
       <c r="B12" s="1" t="s">
         <v>65</v>
       </c>
@@ -1666,7 +1751,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="1" t="s">
         <v>66</v>
       </c>
@@ -1678,7 +1763,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="7"/>
+      <c r="A14" s="8"/>
       <c r="B14" s="1" t="s">
         <v>88</v>
       </c>
@@ -1690,7 +1775,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="7"/>
+      <c r="A15" s="8"/>
       <c r="B15" s="1" t="s">
         <v>19</v>
       </c>
@@ -1705,7 +1790,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="7"/>
+      <c r="A16" s="8"/>
       <c r="B16" s="1" t="s">
         <v>23</v>
       </c>
@@ -1717,7 +1802,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="7"/>
+      <c r="A17" s="8"/>
       <c r="B17" s="1" t="s">
         <v>20</v>
       </c>
@@ -1785,7 +1870,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1800,7 +1885,7 @@
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7"/>
+      <c r="A3" s="8"/>
       <c r="B3" s="1" t="s">
         <v>28</v>
       </c>
@@ -1812,7 +1897,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="1" t="s">
         <v>29</v>
       </c>
@@ -1824,7 +1909,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="1" t="s">
         <v>30</v>
       </c>
@@ -1836,7 +1921,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="1" t="s">
         <v>31</v>
       </c>
@@ -1848,7 +1933,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
+      <c r="A7" s="8"/>
       <c r="B7" s="1" t="s">
         <v>32</v>
       </c>
@@ -1860,7 +1945,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="1" t="s">
         <v>57</v>
       </c>
@@ -1928,7 +2013,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1942,7 +2027,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7"/>
+      <c r="A3" s="8"/>
       <c r="B3" s="1" t="s">
         <v>33</v>
       </c>
@@ -1954,7 +2039,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="1" t="s">
         <v>34</v>
       </c>
@@ -1966,7 +2051,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="1" t="s">
         <v>35</v>
       </c>
@@ -2037,7 +2122,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -2051,7 +2136,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7"/>
+      <c r="A3" s="8"/>
       <c r="B3" s="1" t="s">
         <v>36</v>
       </c>
@@ -2063,7 +2148,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="1" t="s">
         <v>40</v>
       </c>
@@ -2075,7 +2160,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="1" t="s">
         <v>37</v>
       </c>
@@ -2087,7 +2172,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" s="4" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="4" t="s">
         <v>90</v>
       </c>
@@ -2102,7 +2187,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
+      <c r="A7" s="8"/>
       <c r="B7" s="1" t="s">
         <v>38</v>
       </c>
@@ -2114,7 +2199,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="1" t="s">
         <v>39</v>
       </c>
@@ -2126,7 +2211,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="1" t="s">
         <v>91</v>
       </c>
@@ -2138,7 +2223,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
+      <c r="A10" s="8"/>
       <c r="B10" s="1" t="s">
         <v>41</v>
       </c>
@@ -2153,7 +2238,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="7"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="1" t="s">
         <v>42</v>
       </c>
@@ -2165,7 +2250,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="7"/>
+      <c r="A12" s="8"/>
       <c r="B12" s="1" t="s">
         <v>43</v>
       </c>
@@ -2177,7 +2262,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="1" t="s">
         <v>71</v>
       </c>
@@ -2189,7 +2274,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="7"/>
+      <c r="A14" s="8"/>
       <c r="B14" s="1" t="s">
         <v>72</v>
       </c>
@@ -2204,7 +2289,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="7"/>
+      <c r="A15" s="8"/>
       <c r="B15" s="1" t="s">
         <v>73</v>
       </c>
@@ -2272,7 +2357,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -2286,7 +2371,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7"/>
+      <c r="A3" s="8"/>
       <c r="B3" s="1" t="s">
         <v>44</v>
       </c>
@@ -2298,7 +2383,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="1" t="s">
         <v>46</v>
       </c>
@@ -2310,7 +2395,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="1" t="s">
         <v>47</v>
       </c>
@@ -2322,7 +2407,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="1" t="s">
         <v>45</v>
       </c>
@@ -2334,7 +2419,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" s="3" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
+      <c r="A7" s="8"/>
       <c r="B7" s="3" t="s">
         <v>48</v>
       </c>
@@ -2346,7 +2431,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" s="3" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="3" t="s">
         <v>60</v>
       </c>
@@ -2358,7 +2443,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="1" t="s">
         <v>61</v>
       </c>
@@ -2426,7 +2511,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -2440,7 +2525,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7"/>
+      <c r="A3" s="8"/>
       <c r="B3" s="1" t="s">
         <v>49</v>
       </c>
@@ -2452,7 +2537,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="1" t="s">
         <v>50</v>
       </c>
@@ -2464,7 +2549,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="1" t="s">
         <v>58</v>
       </c>
@@ -2476,7 +2561,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="1" t="s">
         <v>59</v>
       </c>
@@ -2488,7 +2573,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
+      <c r="A7" s="8"/>
       <c r="B7" s="1" t="s">
         <v>51</v>
       </c>
@@ -2500,7 +2585,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="1" t="s">
         <v>52</v>
       </c>
@@ -2537,8 +2622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2568,7 +2653,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6"/>
+      <c r="A2" s="7"/>
       <c r="B2" s="1" t="s">
         <v>56</v>
       </c>
@@ -2583,7 +2668,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
+      <c r="A3" s="7"/>
       <c r="B3" s="1" t="s">
         <v>54</v>
       </c>
@@ -2598,7 +2683,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="1" t="s">
         <v>55</v>
       </c>
@@ -2613,7 +2698,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" s="4" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="4" t="s">
         <v>99</v>
       </c>
@@ -2625,7 +2710,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="1" t="s">
         <v>97</v>
       </c>

</xml_diff>